<commit_message>
"minor changes to Bridges.xlsx"
</commit_message>
<xml_diff>
--- a/BridgesLCA/data/Bridges.xlsx
+++ b/BridgesLCA/data/Bridges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/69a54f0becc1d009/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julien.cravero\source\repos\BridgesLCA\BridgesLCA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="8_{65C7C96B-F729-4F1C-97B6-91C21A05654A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{025E3DFF-9FCC-45FE-B939-2F7BB719C1EF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DD3E68-6095-4A28-BE37-7128B28A4CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5762E621-FB6B-4264-B807-B2B391FF7D72}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5762E621-FB6B-4264-B807-B2B391FF7D72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -569,36 +569,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E526AA-CA4F-4250-8712-BF244412D3CB}">
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="33.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" style="2"/>
-    <col min="7" max="7" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.88671875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="25.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="33.75" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.875" style="2"/>
+    <col min="7" max="7" width="10.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,7 +666,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -698,7 +698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -730,7 +730,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -799,7 +799,7 @@
         <v>445500</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -831,7 +831,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -863,7 +863,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -893,7 +893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -923,7 +923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -953,312 +953,312 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22">
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22">
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22">
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22">
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22">
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22">
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22">
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:7">
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:7">
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:7">
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:7">
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:7">
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:7">
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:7">
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:7">
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:7">
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:7">
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:7">
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:7">
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:7">
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:7">
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:7">
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:7">
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:7">
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:7">
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:7">
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:7">
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:7">
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:7">
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:7">
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:7">
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:7">
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:7">
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:7">
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:7">
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:7">
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="5:7">
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="5:7">
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="5:7">
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="5:7">
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:7">
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="5:7">
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
     </row>
-    <row r="52" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:7">
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:7">
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
     </row>
-    <row r="54" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:7">
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
     </row>
-    <row r="55" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="5:7">
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
     </row>
-    <row r="56" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="5:7">
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
     </row>
-    <row r="57" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="5:7">
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="5:7">
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
     </row>
-    <row r="59" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="5:7">
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
     </row>
-    <row r="60" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="5:7">
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
     </row>
-    <row r="61" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="5:7">
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
     </row>
-    <row r="62" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="5:7">
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
     </row>
-    <row r="63" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="5:7">
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
     </row>
-    <row r="64" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="5:7">
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="5:7">
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
     </row>
-    <row r="66" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="5:7">
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
     </row>
-    <row r="67" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="5:7">
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
     </row>
-    <row r="68" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="5:7">
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
     </row>
-    <row r="69" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="5:7">
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
     </row>
-    <row r="70" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="5:7">
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
     </row>
-    <row r="71" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="5:7">
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>

</xml_diff>

<commit_message>
added excel file with some wonderful ratios
</commit_message>
<xml_diff>
--- a/BridgesLCA/data/Bridges.xlsx
+++ b/BridgesLCA/data/Bridges.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/69a54f0becc1d009/Documents/GitHub/BridgesLCA/BridgesLCA/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julien.cravero\source\repos\BridgesLCA\BridgesLCA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{DA8A3E18-6ADE-48B8-BA32-D7D0DEF66817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320204E6-9DC5-47BF-8D84-373908CE3183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5762E621-FB6B-4264-B807-B2B391FF7D72}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{5762E621-FB6B-4264-B807-B2B391FF7D72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -264,13 +263,67 @@
   </si>
   <si>
     <t>16 (C30)</t>
+  </si>
+  <si>
+    <t>Concrete for Piles C30 (m3)</t>
+  </si>
+  <si>
+    <t>Concrete for Foundation C30 (m3)</t>
+  </si>
+  <si>
+    <t>Concrete for Walls and Abutments C30 (m3)</t>
+  </si>
+  <si>
+    <t>Concrete for Piers C30</t>
+  </si>
+  <si>
+    <t>Concrete for Deck C45</t>
+  </si>
+  <si>
+    <t>Concrete for Railings (C30)</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>C30</t>
+  </si>
+  <si>
+    <t>Blinding Concrete C20</t>
+  </si>
+  <si>
+    <t>C45</t>
+  </si>
+  <si>
+    <t>Ratio reinforcement steel/concrete</t>
+  </si>
+  <si>
+    <t>Concrete total (kg)</t>
+  </si>
+  <si>
+    <t>Surface (m2)</t>
+  </si>
+  <si>
+    <t>C20/Surface</t>
+  </si>
+  <si>
+    <t>C30/Surface</t>
+  </si>
+  <si>
+    <t>C45/Surface</t>
+  </si>
+  <si>
+    <t>Structural Steel for Deck/Surface</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,12 +332,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -299,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,6 +381,42 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,34 +753,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E526AA-CA4F-4250-8712-BF244412D3CB}">
   <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="A1:T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="33.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" style="2"/>
-    <col min="7" max="7" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="33.75" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.875" style="2"/>
+    <col min="7" max="7" width="10.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -741,7 +842,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -803,7 +904,7 @@
         <v>78887</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -867,7 +968,7 @@
         <v>320000</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -930,7 +1031,7 @@
         <v>445500</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -984,8 +1085,8 @@
         <v>61</v>
       </c>
       <c r="R5" s="2">
-        <f>136+65</f>
-        <v>201</v>
+        <f>136*65</f>
+        <v>8840</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>55</v>
@@ -995,7 +1096,7 @@
         <v>72881</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -1056,7 +1157,7 @@
         <v>44182</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -1118,7 +1219,7 @@
         <v>88913</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -1180,312 +1281,312 @@
         <v>106481</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20">
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20">
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20">
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20">
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20">
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20">
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20">
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:7">
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:7">
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:7">
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:7">
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:7">
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:7">
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:7">
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:7">
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:7">
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:7">
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:7">
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:7">
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:7">
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:7">
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:7">
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:7">
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:7">
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:7">
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:7">
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:7">
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:7">
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:7">
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:7">
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:7">
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:7">
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:7">
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:7">
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:7">
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:7">
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="5:7">
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="5:7">
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="5:7">
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="5:7">
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:7">
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="5:7">
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
     </row>
-    <row r="52" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:7">
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:7">
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
     </row>
-    <row r="54" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:7">
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
     </row>
-    <row r="55" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="5:7">
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
     </row>
-    <row r="56" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="5:7">
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
     </row>
-    <row r="57" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="5:7">
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="5:7">
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
     </row>
-    <row r="59" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="5:7">
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
     </row>
-    <row r="60" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="5:7">
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
     </row>
-    <row r="61" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="5:7">
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
     </row>
-    <row r="62" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="5:7">
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
     </row>
-    <row r="63" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="5:7">
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
     </row>
-    <row r="64" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="5:7">
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="5:7">
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
     </row>
-    <row r="66" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="5:7">
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
     </row>
-    <row r="67" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="5:7">
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
     </row>
-    <row r="68" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="5:7">
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
     </row>
-    <row r="69" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="5:7">
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
     </row>
-    <row r="70" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="5:7">
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -1496,4 +1597,854 @@
     <ignoredError sqref="C2:C4 C5:C8" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD34624-FC8C-460F-B69E-766DA3D31091}">
+  <dimension ref="A1:AD10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+      <selection activeCell="Y10" sqref="Y10:Y14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.25" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.25" customWidth="1"/>
+    <col min="25" max="25" width="29.25" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3">
+        <v>44</v>
+      </c>
+      <c r="F2" s="3">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2">
+        <v>85</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>149</v>
+      </c>
+      <c r="M2" s="2">
+        <v>54</v>
+      </c>
+      <c r="N2" s="2">
+        <v>200</v>
+      </c>
+      <c r="O2" s="2">
+        <v>283</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>12090</v>
+      </c>
+      <c r="S2" s="2">
+        <v>185</v>
+      </c>
+      <c r="T2" s="2">
+        <v>78887</v>
+      </c>
+      <c r="U2">
+        <f>S2</f>
+        <v>185</v>
+      </c>
+      <c r="V2">
+        <f>J2+L2+M2+N2</f>
+        <v>488</v>
+      </c>
+      <c r="W2">
+        <f>O2</f>
+        <v>283</v>
+      </c>
+      <c r="X2">
+        <f>(U2+V2+W2)*2400</f>
+        <v>2294400</v>
+      </c>
+      <c r="Y2" s="6">
+        <f>2400*T2/X2</f>
+        <v>82.51778242677824</v>
+      </c>
+      <c r="Z2">
+        <f>E2*F2</f>
+        <v>484</v>
+      </c>
+      <c r="AA2" s="6">
+        <f>U2/Z2</f>
+        <v>0.38223140495867769</v>
+      </c>
+      <c r="AB2" s="6">
+        <f>V2/Z2</f>
+        <v>1.0082644628099173</v>
+      </c>
+      <c r="AC2" s="6">
+        <f>W2/Z2</f>
+        <v>0.58471074380165289</v>
+      </c>
+      <c r="AD2">
+        <f>P2/Z2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3">
+        <v>46</v>
+      </c>
+      <c r="F3" s="3">
+        <v>36</v>
+      </c>
+      <c r="G3" s="3">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>11</v>
+      </c>
+      <c r="J3" s="2">
+        <v>202</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>596</v>
+      </c>
+      <c r="M3" s="2">
+        <v>36</v>
+      </c>
+      <c r="N3" s="2">
+        <v>300</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1230</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <f>99.6*65</f>
+        <v>6474</v>
+      </c>
+      <c r="S3" s="2">
+        <v>202</v>
+      </c>
+      <c r="T3" s="2">
+        <f>276000+44000</f>
+        <v>320000</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U8" si="0">S3</f>
+        <v>202</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V8" si="1">J3+L3+M3+N3</f>
+        <v>1134</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W8" si="2">O3</f>
+        <v>1230</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X8" si="3">(U3+V3+W3)*2400</f>
+        <v>6158400</v>
+      </c>
+      <c r="Y3" s="6">
+        <f t="shared" ref="Y3:Y8" si="4">2400*T3/X3</f>
+        <v>124.70771628994544</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z8" si="5">E3*F3</f>
+        <v>1656</v>
+      </c>
+      <c r="AA3" s="6">
+        <f t="shared" ref="AA3:AA8" si="6">U3/Z3</f>
+        <v>0.12198067632850242</v>
+      </c>
+      <c r="AB3" s="6">
+        <f t="shared" ref="AB3:AB8" si="7">V3/Z3</f>
+        <v>0.68478260869565222</v>
+      </c>
+      <c r="AC3" s="6">
+        <f t="shared" ref="AC3:AC8" si="8">W3/Z3</f>
+        <v>0.74275362318840576</v>
+      </c>
+      <c r="AD3">
+        <f>P3/Z3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" s="19" customFormat="1">
+      <c r="A4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="17">
+        <v>80</v>
+      </c>
+      <c r="F4" s="17">
+        <v>22</v>
+      </c>
+      <c r="G4" s="17">
+        <v>11</v>
+      </c>
+      <c r="H4" s="18">
+        <v>3</v>
+      </c>
+      <c r="I4" s="18">
+        <v>19</v>
+      </c>
+      <c r="J4" s="18">
+        <v>0</v>
+      </c>
+      <c r="K4" s="18">
+        <v>135700</v>
+      </c>
+      <c r="L4" s="18">
+        <v>711</v>
+      </c>
+      <c r="M4" s="18">
+        <v>129</v>
+      </c>
+      <c r="N4" s="18">
+        <v>773</v>
+      </c>
+      <c r="O4" s="18">
+        <v>864</v>
+      </c>
+      <c r="P4" s="18">
+        <v>373500</v>
+      </c>
+      <c r="Q4" s="18">
+        <v>0</v>
+      </c>
+      <c r="R4" s="18">
+        <v>19000</v>
+      </c>
+      <c r="S4" s="18">
+        <v>604</v>
+      </c>
+      <c r="T4" s="18">
+        <f>175000+110000+160500</f>
+        <v>445500</v>
+      </c>
+      <c r="U4" s="19">
+        <f t="shared" si="0"/>
+        <v>604</v>
+      </c>
+      <c r="V4" s="19">
+        <f t="shared" si="1"/>
+        <v>1613</v>
+      </c>
+      <c r="W4" s="19">
+        <f t="shared" si="2"/>
+        <v>864</v>
+      </c>
+      <c r="X4" s="19">
+        <f t="shared" si="3"/>
+        <v>7394400</v>
+      </c>
+      <c r="Y4" s="20">
+        <f t="shared" si="4"/>
+        <v>144.59591041869524</v>
+      </c>
+      <c r="Z4" s="19">
+        <f t="shared" si="5"/>
+        <v>1760</v>
+      </c>
+      <c r="AA4" s="20">
+        <f t="shared" si="6"/>
+        <v>0.3431818181818182</v>
+      </c>
+      <c r="AB4" s="20">
+        <f t="shared" si="7"/>
+        <v>0.91647727272727275</v>
+      </c>
+      <c r="AC4" s="20">
+        <f t="shared" si="8"/>
+        <v>0.49090909090909091</v>
+      </c>
+      <c r="AD4" s="21">
+        <f t="shared" ref="AD4:AD8" si="9">P4/Z4</f>
+        <v>212.21590909090909</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3">
+        <v>51.5</v>
+      </c>
+      <c r="F5" s="3">
+        <v>9.6</v>
+      </c>
+      <c r="G5" s="3">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>6</v>
+      </c>
+      <c r="J5" s="2">
+        <v>119</v>
+      </c>
+      <c r="K5" s="2">
+        <f>2731+428</f>
+        <v>3159</v>
+      </c>
+      <c r="L5" s="2">
+        <v>70</v>
+      </c>
+      <c r="M5" s="2">
+        <v>188</v>
+      </c>
+      <c r="N5" s="2">
+        <v>63</v>
+      </c>
+      <c r="O5" s="2">
+        <v>365</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>20</v>
+      </c>
+      <c r="R5" s="2">
+        <f>136*65</f>
+        <v>8840</v>
+      </c>
+      <c r="S5" s="2">
+        <v>37</v>
+      </c>
+      <c r="T5" s="2">
+        <f>14165+57050+1666</f>
+        <v>72881</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="1"/>
+        <v>440</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="2"/>
+        <v>365</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="3"/>
+        <v>2020800</v>
+      </c>
+      <c r="Y5" s="6">
+        <f t="shared" si="4"/>
+        <v>86.557007125890735</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="5"/>
+        <v>494.4</v>
+      </c>
+      <c r="AA5" s="6">
+        <f t="shared" si="6"/>
+        <v>7.4838187702265371E-2</v>
+      </c>
+      <c r="AB5" s="6">
+        <f t="shared" si="7"/>
+        <v>0.88996763754045316</v>
+      </c>
+      <c r="AC5" s="6">
+        <f t="shared" si="8"/>
+        <v>0.73826860841423947</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" s="12" customFormat="1">
+      <c r="A6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="10">
+        <v>7.7</v>
+      </c>
+      <c r="F6" s="10">
+        <v>16.2</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11">
+        <v>1</v>
+      </c>
+      <c r="I6" s="11">
+        <v>3</v>
+      </c>
+      <c r="J6" s="11">
+        <v>2</v>
+      </c>
+      <c r="K6" s="11">
+        <v>0</v>
+      </c>
+      <c r="L6" s="11">
+        <v>66</v>
+      </c>
+      <c r="M6" s="11">
+        <v>34</v>
+      </c>
+      <c r="N6" s="11">
+        <v>0</v>
+      </c>
+      <c r="O6" s="11">
+        <v>151</v>
+      </c>
+      <c r="P6" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>0</v>
+      </c>
+      <c r="R6" s="11">
+        <f>27*65</f>
+        <v>1755</v>
+      </c>
+      <c r="S6" s="11">
+        <v>24</v>
+      </c>
+      <c r="T6" s="11">
+        <v>44182</v>
+      </c>
+      <c r="U6" s="12">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="V6" s="12">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="W6" s="12">
+        <f t="shared" si="2"/>
+        <v>151</v>
+      </c>
+      <c r="X6" s="12">
+        <f t="shared" si="3"/>
+        <v>664800</v>
+      </c>
+      <c r="Y6" s="13">
+        <f t="shared" si="4"/>
+        <v>159.50180505415162</v>
+      </c>
+      <c r="Z6" s="12">
+        <f t="shared" si="5"/>
+        <v>124.74</v>
+      </c>
+      <c r="AA6" s="13">
+        <f t="shared" si="6"/>
+        <v>0.1924001924001924</v>
+      </c>
+      <c r="AB6" s="13">
+        <f t="shared" si="7"/>
+        <v>0.81770081770081771</v>
+      </c>
+      <c r="AC6" s="13">
+        <f t="shared" si="8"/>
+        <v>1.210517877184544</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30">
+      <c r="A7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3">
+        <v>44.8</v>
+      </c>
+      <c r="F7" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="2">
+        <v>2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>6</v>
+      </c>
+      <c r="J7" s="2">
+        <v>16</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>95</v>
+      </c>
+      <c r="M7" s="2">
+        <v>134</v>
+      </c>
+      <c r="N7" s="2">
+        <v>34</v>
+      </c>
+      <c r="O7" s="2">
+        <v>443</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2">
+        <f>99.6*65</f>
+        <v>6474</v>
+      </c>
+      <c r="S7" s="2">
+        <v>32</v>
+      </c>
+      <c r="T7" s="2">
+        <f>73958+14955</f>
+        <v>88913</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="1"/>
+        <v>279</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="2"/>
+        <v>443</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="3"/>
+        <v>1809600</v>
+      </c>
+      <c r="Y7" s="6">
+        <f t="shared" si="4"/>
+        <v>117.92175066312997</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="5"/>
+        <v>560</v>
+      </c>
+      <c r="AA7" s="6">
+        <f t="shared" si="6"/>
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="AB7" s="6">
+        <f t="shared" si="7"/>
+        <v>0.49821428571428572</v>
+      </c>
+      <c r="AC7" s="6">
+        <f t="shared" si="8"/>
+        <v>0.79107142857142854</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30">
+      <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3">
+        <v>47.5</v>
+      </c>
+      <c r="F8" s="3">
+        <v>12.8</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="2">
+        <v>2</v>
+      </c>
+      <c r="I8" s="2">
+        <v>6</v>
+      </c>
+      <c r="J8" s="2">
+        <v>36</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>111</v>
+      </c>
+      <c r="M8" s="2">
+        <v>129</v>
+      </c>
+      <c r="N8" s="2">
+        <v>43</v>
+      </c>
+      <c r="O8" s="2">
+        <v>483</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <f>105*65</f>
+        <v>6825</v>
+      </c>
+      <c r="S8" s="2">
+        <v>29</v>
+      </c>
+      <c r="T8" s="2">
+        <f>88654+17827</f>
+        <v>106481</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="1"/>
+        <v>319</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="2"/>
+        <v>483</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="3"/>
+        <v>1994400</v>
+      </c>
+      <c r="Y8" s="6">
+        <f t="shared" si="4"/>
+        <v>128.13598074608905</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="5"/>
+        <v>608</v>
+      </c>
+      <c r="AA8" s="6">
+        <f t="shared" si="6"/>
+        <v>4.7697368421052634E-2</v>
+      </c>
+      <c r="AB8" s="6">
+        <f t="shared" si="7"/>
+        <v>0.52467105263157898</v>
+      </c>
+      <c r="AC8" s="6">
+        <f t="shared" si="8"/>
+        <v>0.79440789473684215</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30">
+      <c r="Y10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bridges excel file with data on the first sheet bridges_data
</commit_message>
<xml_diff>
--- a/BridgesLCA/data/Bridges.xlsx
+++ b/BridgesLCA/data/Bridges.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julien.cravero\source\repos\BridgesLCA\BridgesLCA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320204E6-9DC5-47BF-8D84-373908CE3183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EFD877-7439-44F1-BDF8-7DB7DDF3A67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{5762E621-FB6B-4264-B807-B2B391FF7D72}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5762E621-FB6B-4264-B807-B2B391FF7D72}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
+    <sheet name="bridges_data" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Feuil1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="105">
   <si>
     <t>Name</t>
   </si>
@@ -265,24 +266,12 @@
     <t>16 (C30)</t>
   </si>
   <si>
-    <t>Concrete for Piles C30 (m3)</t>
-  </si>
-  <si>
-    <t>Concrete for Foundation C30 (m3)</t>
-  </si>
-  <si>
-    <t>Concrete for Walls and Abutments C30 (m3)</t>
-  </si>
-  <si>
     <t>Concrete for Piers C30</t>
   </si>
   <si>
     <t>Concrete for Deck C45</t>
   </si>
   <si>
-    <t>Concrete for Railings (C30)</t>
-  </si>
-  <si>
     <t>C20</t>
   </si>
   <si>
@@ -314,6 +303,54 @@
   </si>
   <si>
     <t>Structural Steel for Deck/Surface</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Maximum Height</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Duration of Installation</t>
+  </si>
+  <si>
+    <t>months</t>
+  </si>
+  <si>
+    <t>Concrete for Piles C30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> m3</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Structural Steel for Piles</t>
+  </si>
+  <si>
+    <t>Concrete for Foundations C30</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>Concrete for Walls and Abutments C30</t>
+  </si>
+  <si>
+    <t>Concrete for Railings C302</t>
+  </si>
+  <si>
+    <t>Reinforcing Steel</t>
   </si>
 </sst>
 </file>
@@ -321,7 +358,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -381,7 +418,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -398,7 +435,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -415,7 +452,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -750,6 +787,576 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10924730-7B98-45F4-B23C-B5F7ED65DD7F}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3">
+        <v>44</v>
+      </c>
+      <c r="F3" s="3">
+        <v>11</v>
+      </c>
+      <c r="G3" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="H3" s="2">
+        <v>3</v>
+      </c>
+      <c r="I3" s="2">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2">
+        <v>85</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>149</v>
+      </c>
+      <c r="M3" s="2">
+        <v>54</v>
+      </c>
+      <c r="N3" s="2">
+        <v>200</v>
+      </c>
+      <c r="O3" s="2">
+        <v>283</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>12090</v>
+      </c>
+      <c r="S3" s="2">
+        <v>185</v>
+      </c>
+      <c r="T3" s="2">
+        <v>78887</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3">
+        <v>46</v>
+      </c>
+      <c r="F4" s="3">
+        <v>36</v>
+      </c>
+      <c r="G4" s="3">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>11</v>
+      </c>
+      <c r="J4" s="2">
+        <v>202</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>596</v>
+      </c>
+      <c r="M4" s="2">
+        <v>36</v>
+      </c>
+      <c r="N4" s="2">
+        <v>300</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1230</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <f>99.6*65</f>
+        <v>6474</v>
+      </c>
+      <c r="S4" s="2">
+        <v>202</v>
+      </c>
+      <c r="T4" s="2">
+        <f>276000+44000</f>
+        <v>320000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="17">
+        <v>80</v>
+      </c>
+      <c r="F5" s="17">
+        <v>22</v>
+      </c>
+      <c r="G5" s="17">
+        <v>11</v>
+      </c>
+      <c r="H5" s="18">
+        <v>3</v>
+      </c>
+      <c r="I5" s="18">
+        <v>19</v>
+      </c>
+      <c r="J5" s="18">
+        <v>0</v>
+      </c>
+      <c r="K5" s="18">
+        <v>135700</v>
+      </c>
+      <c r="L5" s="18">
+        <v>711</v>
+      </c>
+      <c r="M5" s="18">
+        <v>129</v>
+      </c>
+      <c r="N5" s="18">
+        <v>773</v>
+      </c>
+      <c r="O5" s="18">
+        <v>864</v>
+      </c>
+      <c r="P5" s="18">
+        <v>373500</v>
+      </c>
+      <c r="Q5" s="18">
+        <v>0</v>
+      </c>
+      <c r="R5" s="18">
+        <v>19000</v>
+      </c>
+      <c r="S5" s="18">
+        <v>604</v>
+      </c>
+      <c r="T5" s="18">
+        <f>175000+110000+160500</f>
+        <v>445500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3">
+        <v>51.5</v>
+      </c>
+      <c r="F6" s="3">
+        <v>9.6</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>6</v>
+      </c>
+      <c r="J6" s="2">
+        <v>119</v>
+      </c>
+      <c r="K6" s="2">
+        <f>2731+428</f>
+        <v>3159</v>
+      </c>
+      <c r="L6" s="2">
+        <v>70</v>
+      </c>
+      <c r="M6" s="2">
+        <v>188</v>
+      </c>
+      <c r="N6" s="2">
+        <v>63</v>
+      </c>
+      <c r="O6" s="2">
+        <v>365</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>20</v>
+      </c>
+      <c r="R6" s="2">
+        <f>136*65</f>
+        <v>8840</v>
+      </c>
+      <c r="S6" s="2">
+        <v>37</v>
+      </c>
+      <c r="T6" s="2">
+        <f>14165+57050+1666</f>
+        <v>72881</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="10">
+        <v>7.7</v>
+      </c>
+      <c r="F7" s="10">
+        <v>16.2</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="11">
+        <v>1</v>
+      </c>
+      <c r="I7" s="11">
+        <v>3</v>
+      </c>
+      <c r="J7" s="11">
+        <v>2</v>
+      </c>
+      <c r="K7" s="11">
+        <v>0</v>
+      </c>
+      <c r="L7" s="11">
+        <v>66</v>
+      </c>
+      <c r="M7" s="11">
+        <v>34</v>
+      </c>
+      <c r="N7" s="11">
+        <v>0</v>
+      </c>
+      <c r="O7" s="11">
+        <v>151</v>
+      </c>
+      <c r="P7" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>0</v>
+      </c>
+      <c r="R7" s="11">
+        <f>27*65</f>
+        <v>1755</v>
+      </c>
+      <c r="S7" s="11">
+        <v>24</v>
+      </c>
+      <c r="T7" s="11">
+        <v>44182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3">
+        <v>44.8</v>
+      </c>
+      <c r="F8" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="2">
+        <v>2</v>
+      </c>
+      <c r="I8" s="2">
+        <v>6</v>
+      </c>
+      <c r="J8" s="2">
+        <v>16</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>95</v>
+      </c>
+      <c r="M8" s="2">
+        <v>134</v>
+      </c>
+      <c r="N8" s="2">
+        <v>34</v>
+      </c>
+      <c r="O8" s="2">
+        <v>443</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <f>99.6*65</f>
+        <v>6474</v>
+      </c>
+      <c r="S8" s="2">
+        <v>32</v>
+      </c>
+      <c r="T8" s="2">
+        <f>73958+14955</f>
+        <v>88913</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3">
+        <v>47.5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12.8</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>6</v>
+      </c>
+      <c r="J9" s="2">
+        <v>36</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>111</v>
+      </c>
+      <c r="M9" s="2">
+        <v>129</v>
+      </c>
+      <c r="N9" s="2">
+        <v>43</v>
+      </c>
+      <c r="O9" s="2">
+        <v>483</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2">
+        <f>105*65</f>
+        <v>6825</v>
+      </c>
+      <c r="S9" s="2">
+        <v>29</v>
+      </c>
+      <c r="T9" s="2">
+        <f>88654+17827</f>
+        <v>106481</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E526AA-CA4F-4250-8712-BF244412D3CB}">
   <dimension ref="A1:T70"/>
   <sheetViews>
@@ -1599,18 +2206,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD34624-FC8C-460F-B69E-766DA3D31091}">
-  <dimension ref="A1:AD10"/>
+  <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10:Y14"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="T9" sqref="A1:T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.75" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
@@ -1644,696 +2252,658 @@
         <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>29</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>31</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="W1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="Y1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="AA1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:30">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD1" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:30">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3">
-        <v>44</v>
-      </c>
-      <c r="F2" s="3">
-        <v>11</v>
-      </c>
-      <c r="G2" s="3">
-        <v>7.8</v>
-      </c>
-      <c r="H2" s="2">
-        <v>3</v>
-      </c>
-      <c r="I2" s="2">
-        <v>7</v>
-      </c>
-      <c r="J2" s="2">
-        <v>85</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>149</v>
-      </c>
-      <c r="M2" s="2">
-        <v>54</v>
-      </c>
-      <c r="N2" s="2">
-        <v>200</v>
-      </c>
-      <c r="O2" s="2">
-        <v>283</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0</v>
-      </c>
-      <c r="R2" s="2">
-        <v>12090</v>
-      </c>
-      <c r="S2" s="2">
-        <v>185</v>
-      </c>
-      <c r="T2" s="2">
-        <v>78887</v>
-      </c>
-      <c r="U2">
-        <f>S2</f>
-        <v>185</v>
-      </c>
-      <c r="V2">
-        <f>J2+L2+M2+N2</f>
-        <v>488</v>
-      </c>
-      <c r="W2">
-        <f>O2</f>
-        <v>283</v>
-      </c>
-      <c r="X2">
-        <f>(U2+V2+W2)*2400</f>
-        <v>2294400</v>
-      </c>
-      <c r="Y2" s="6">
-        <f>2400*T2/X2</f>
-        <v>82.51778242677824</v>
-      </c>
-      <c r="Z2">
-        <f>E2*F2</f>
-        <v>484</v>
-      </c>
-      <c r="AA2" s="6">
-        <f>U2/Z2</f>
-        <v>0.38223140495867769</v>
-      </c>
-      <c r="AB2" s="6">
-        <f>V2/Z2</f>
-        <v>1.0082644628099173</v>
-      </c>
-      <c r="AC2" s="6">
-        <f>W2/Z2</f>
-        <v>0.58471074380165289</v>
-      </c>
-      <c r="AD2">
-        <f>P2/Z2</f>
-        <v>0</v>
-      </c>
+      <c r="H2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
     </row>
     <row r="3" spans="1:30">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="3">
+        <v>44</v>
+      </c>
+      <c r="F3" s="3">
+        <v>11</v>
+      </c>
+      <c r="G3" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="H3" s="2">
+        <v>3</v>
+      </c>
+      <c r="I3" s="2">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2">
+        <v>85</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>149</v>
+      </c>
+      <c r="M3" s="2">
+        <v>54</v>
+      </c>
+      <c r="N3" s="2">
+        <v>200</v>
+      </c>
+      <c r="O3" s="2">
+        <v>283</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>12090</v>
+      </c>
+      <c r="S3" s="2">
+        <v>185</v>
+      </c>
+      <c r="T3" s="2">
+        <v>78887</v>
+      </c>
+      <c r="U3">
+        <f>S3</f>
+        <v>185</v>
+      </c>
+      <c r="V3">
+        <f>J3+L3+M3+N3</f>
+        <v>488</v>
+      </c>
+      <c r="W3">
+        <f>O3</f>
+        <v>283</v>
+      </c>
+      <c r="X3">
+        <f>(U3+V3+W3)*2400</f>
+        <v>2294400</v>
+      </c>
+      <c r="Y3" s="6">
+        <f>2400*T3/X3</f>
+        <v>82.51778242677824</v>
+      </c>
+      <c r="Z3">
+        <f>E3*F3</f>
+        <v>484</v>
+      </c>
+      <c r="AA3" s="6">
+        <f>U3/Z3</f>
+        <v>0.38223140495867769</v>
+      </c>
+      <c r="AB3" s="6">
+        <f>V3/Z3</f>
+        <v>1.0082644628099173</v>
+      </c>
+      <c r="AC3" s="6">
+        <f>W3/Z3</f>
+        <v>0.58471074380165289</v>
+      </c>
+      <c r="AD3">
+        <f>P3/Z3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3">
         <v>46</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F4" s="3">
         <v>36</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G4" s="3">
         <v>10</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H4" s="2">
         <v>2</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I4" s="2">
         <v>11</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J4" s="2">
         <v>202</v>
       </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
         <v>596</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M4" s="2">
         <v>36</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N4" s="2">
         <v>300</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O4" s="2">
         <v>1230</v>
       </c>
-      <c r="P3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0</v>
-      </c>
-      <c r="R3" s="2">
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
         <f>99.6*65</f>
         <v>6474</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S4" s="2">
         <v>202</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T4" s="2">
         <f>276000+44000</f>
         <v>320000</v>
       </c>
-      <c r="U3">
-        <f t="shared" ref="U3:U8" si="0">S3</f>
+      <c r="U4">
+        <f t="shared" ref="U4:U9" si="0">S4</f>
         <v>202</v>
       </c>
-      <c r="V3">
-        <f t="shared" ref="V3:V8" si="1">J3+L3+M3+N3</f>
+      <c r="V4">
+        <f t="shared" ref="V4:V9" si="1">J4+L4+M4+N4</f>
         <v>1134</v>
       </c>
-      <c r="W3">
-        <f t="shared" ref="W3:W8" si="2">O3</f>
+      <c r="W4">
+        <f t="shared" ref="W4:W9" si="2">O4</f>
         <v>1230</v>
       </c>
-      <c r="X3">
-        <f t="shared" ref="X3:X8" si="3">(U3+V3+W3)*2400</f>
+      <c r="X4">
+        <f t="shared" ref="X4:X9" si="3">(U4+V4+W4)*2400</f>
         <v>6158400</v>
       </c>
-      <c r="Y3" s="6">
-        <f t="shared" ref="Y3:Y8" si="4">2400*T3/X3</f>
+      <c r="Y4" s="6">
+        <f t="shared" ref="Y4:Y9" si="4">2400*T4/X4</f>
         <v>124.70771628994544</v>
       </c>
-      <c r="Z3">
-        <f t="shared" ref="Z3:Z8" si="5">E3*F3</f>
+      <c r="Z4">
+        <f t="shared" ref="Z4:Z9" si="5">E4*F4</f>
         <v>1656</v>
       </c>
-      <c r="AA3" s="6">
-        <f t="shared" ref="AA3:AA8" si="6">U3/Z3</f>
+      <c r="AA4" s="6">
+        <f t="shared" ref="AA4:AA9" si="6">U4/Z4</f>
         <v>0.12198067632850242</v>
       </c>
-      <c r="AB3" s="6">
-        <f t="shared" ref="AB3:AB8" si="7">V3/Z3</f>
+      <c r="AB4" s="6">
+        <f t="shared" ref="AB4:AB9" si="7">V4/Z4</f>
         <v>0.68478260869565222</v>
       </c>
-      <c r="AC3" s="6">
-        <f t="shared" ref="AC3:AC8" si="8">W3/Z3</f>
+      <c r="AC4" s="6">
+        <f t="shared" ref="AC4:AC9" si="8">W4/Z4</f>
         <v>0.74275362318840576</v>
       </c>
-      <c r="AD3">
-        <f>P3/Z3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" s="19" customFormat="1">
-      <c r="A4" s="14" t="s">
+      <c r="AD4">
+        <f>P4/Z4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" s="19" customFormat="1">
+      <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E5" s="17">
         <v>80</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F5" s="17">
         <v>22</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G5" s="17">
         <v>11</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H5" s="18">
         <v>3</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I5" s="18">
         <v>19</v>
       </c>
-      <c r="J4" s="18">
-        <v>0</v>
-      </c>
-      <c r="K4" s="18">
+      <c r="J5" s="18">
+        <v>0</v>
+      </c>
+      <c r="K5" s="18">
         <v>135700</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L5" s="18">
         <v>711</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M5" s="18">
         <v>129</v>
       </c>
-      <c r="N4" s="18">
+      <c r="N5" s="18">
         <v>773</v>
       </c>
-      <c r="O4" s="18">
+      <c r="O5" s="18">
         <v>864</v>
       </c>
-      <c r="P4" s="18">
+      <c r="P5" s="18">
         <v>373500</v>
       </c>
-      <c r="Q4" s="18">
-        <v>0</v>
-      </c>
-      <c r="R4" s="18">
+      <c r="Q5" s="18">
+        <v>0</v>
+      </c>
+      <c r="R5" s="18">
         <v>19000</v>
       </c>
-      <c r="S4" s="18">
+      <c r="S5" s="18">
         <v>604</v>
       </c>
-      <c r="T4" s="18">
+      <c r="T5" s="18">
         <f>175000+110000+160500</f>
         <v>445500</v>
       </c>
-      <c r="U4" s="19">
+      <c r="U5" s="19">
         <f t="shared" si="0"/>
         <v>604</v>
       </c>
-      <c r="V4" s="19">
+      <c r="V5" s="19">
         <f t="shared" si="1"/>
         <v>1613</v>
       </c>
-      <c r="W4" s="19">
+      <c r="W5" s="19">
         <f t="shared" si="2"/>
         <v>864</v>
       </c>
-      <c r="X4" s="19">
+      <c r="X5" s="19">
         <f t="shared" si="3"/>
         <v>7394400</v>
       </c>
-      <c r="Y4" s="20">
+      <c r="Y5" s="20">
         <f t="shared" si="4"/>
         <v>144.59591041869524</v>
       </c>
-      <c r="Z4" s="19">
+      <c r="Z5" s="19">
         <f t="shared" si="5"/>
         <v>1760</v>
       </c>
-      <c r="AA4" s="20">
+      <c r="AA5" s="20">
         <f t="shared" si="6"/>
         <v>0.3431818181818182</v>
       </c>
-      <c r="AB4" s="20">
+      <c r="AB5" s="20">
         <f t="shared" si="7"/>
         <v>0.91647727272727275</v>
       </c>
-      <c r="AC4" s="20">
+      <c r="AC5" s="20">
         <f t="shared" si="8"/>
         <v>0.49090909090909091</v>
       </c>
-      <c r="AD4" s="21">
-        <f t="shared" ref="AD4:AD8" si="9">P4/Z4</f>
+      <c r="AD5" s="21">
+        <f t="shared" ref="AD5:AD9" si="9">P5/Z5</f>
         <v>212.21590909090909</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:30">
+      <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E6" s="3">
         <v>51.5</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F6" s="3">
         <v>9.6</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G6" s="3">
         <v>5</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H6" s="2">
         <v>2</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I6" s="2">
         <v>6</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J6" s="2">
         <v>119</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K6" s="2">
         <f>2731+428</f>
         <v>3159</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L6" s="2">
         <v>70</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M6" s="2">
         <v>188</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N6" s="2">
         <v>63</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O6" s="2">
         <v>365</v>
       </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
         <v>20</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R6" s="2">
         <f>136*65</f>
         <v>8840</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S6" s="2">
         <v>37</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T6" s="2">
         <f>14165+57050+1666</f>
         <v>72881</v>
       </c>
-      <c r="U5">
+      <c r="U6">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="V5">
+      <c r="V6">
         <f t="shared" si="1"/>
         <v>440</v>
       </c>
-      <c r="W5">
+      <c r="W6">
         <f t="shared" si="2"/>
         <v>365</v>
       </c>
-      <c r="X5">
+      <c r="X6">
         <f t="shared" si="3"/>
         <v>2020800</v>
       </c>
-      <c r="Y5" s="6">
+      <c r="Y6" s="6">
         <f t="shared" si="4"/>
         <v>86.557007125890735</v>
       </c>
-      <c r="Z5">
+      <c r="Z6">
         <f t="shared" si="5"/>
         <v>494.4</v>
       </c>
-      <c r="AA5" s="6">
+      <c r="AA6" s="6">
         <f t="shared" si="6"/>
         <v>7.4838187702265371E-2</v>
       </c>
-      <c r="AB5" s="6">
+      <c r="AB6" s="6">
         <f t="shared" si="7"/>
         <v>0.88996763754045316</v>
       </c>
-      <c r="AC5" s="6">
+      <c r="AC6" s="6">
         <f t="shared" si="8"/>
         <v>0.73826860841423947</v>
       </c>
-      <c r="AD5">
+      <c r="AD6">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="12" customFormat="1">
-      <c r="A6" s="7" t="s">
+    <row r="7" spans="1:30" s="12" customFormat="1">
+      <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E7" s="10">
         <v>7.7</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F7" s="10">
         <v>16.2</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11">
+      <c r="G7" s="10"/>
+      <c r="H7" s="11">
         <v>1</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I7" s="11">
         <v>3</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J7" s="11">
         <v>2</v>
       </c>
-      <c r="K6" s="11">
-        <v>0</v>
-      </c>
-      <c r="L6" s="11">
+      <c r="K7" s="11">
+        <v>0</v>
+      </c>
+      <c r="L7" s="11">
         <v>66</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M7" s="11">
         <v>34</v>
       </c>
-      <c r="N6" s="11">
-        <v>0</v>
-      </c>
-      <c r="O6" s="11">
+      <c r="N7" s="11">
+        <v>0</v>
+      </c>
+      <c r="O7" s="11">
         <v>151</v>
       </c>
-      <c r="P6" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="11">
-        <v>0</v>
-      </c>
-      <c r="R6" s="11">
+      <c r="P7" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>0</v>
+      </c>
+      <c r="R7" s="11">
         <f>27*65</f>
         <v>1755</v>
       </c>
-      <c r="S6" s="11">
+      <c r="S7" s="11">
         <v>24</v>
       </c>
-      <c r="T6" s="11">
+      <c r="T7" s="11">
         <v>44182</v>
       </c>
-      <c r="U6" s="12">
+      <c r="U7" s="12">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="V6" s="12">
+      <c r="V7" s="12">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
-      <c r="W6" s="12">
+      <c r="W7" s="12">
         <f t="shared" si="2"/>
         <v>151</v>
       </c>
-      <c r="X6" s="12">
+      <c r="X7" s="12">
         <f t="shared" si="3"/>
         <v>664800</v>
       </c>
-      <c r="Y6" s="13">
+      <c r="Y7" s="13">
         <f t="shared" si="4"/>
         <v>159.50180505415162</v>
       </c>
-      <c r="Z6" s="12">
+      <c r="Z7" s="12">
         <f t="shared" si="5"/>
         <v>124.74</v>
       </c>
-      <c r="AA6" s="13">
+      <c r="AA7" s="13">
         <f t="shared" si="6"/>
         <v>0.1924001924001924</v>
       </c>
-      <c r="AB6" s="13">
+      <c r="AB7" s="13">
         <f t="shared" si="7"/>
         <v>0.81770081770081771</v>
       </c>
-      <c r="AC6" s="13">
+      <c r="AC7" s="13">
         <f t="shared" si="8"/>
         <v>1.210517877184544</v>
       </c>
-      <c r="AD6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30">
-      <c r="A7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="3">
-        <v>44.8</v>
-      </c>
-      <c r="F7" s="3">
-        <v>12.5</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="2">
-        <v>2</v>
-      </c>
-      <c r="I7" s="2">
-        <v>6</v>
-      </c>
-      <c r="J7" s="2">
-        <v>16</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2">
-        <v>95</v>
-      </c>
-      <c r="M7" s="2">
-        <v>134</v>
-      </c>
-      <c r="N7" s="2">
-        <v>34</v>
-      </c>
-      <c r="O7" s="2">
-        <v>443</v>
-      </c>
-      <c r="P7" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>0</v>
-      </c>
-      <c r="R7" s="2">
-        <f>99.6*65</f>
-        <v>6474</v>
-      </c>
-      <c r="S7" s="2">
-        <v>32</v>
-      </c>
-      <c r="T7" s="2">
-        <f>73958+14955</f>
-        <v>88913</v>
-      </c>
-      <c r="U7">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="V7">
-        <f t="shared" si="1"/>
-        <v>279</v>
-      </c>
-      <c r="W7">
-        <f t="shared" si="2"/>
-        <v>443</v>
-      </c>
-      <c r="X7">
-        <f t="shared" si="3"/>
-        <v>1809600</v>
-      </c>
-      <c r="Y7" s="6">
-        <f t="shared" si="4"/>
-        <v>117.92175066312997</v>
-      </c>
-      <c r="Z7">
-        <f t="shared" si="5"/>
-        <v>560</v>
-      </c>
-      <c r="AA7" s="6">
-        <f t="shared" si="6"/>
-        <v>5.7142857142857141E-2</v>
-      </c>
-      <c r="AB7" s="6">
-        <f t="shared" si="7"/>
-        <v>0.49821428571428572</v>
-      </c>
-      <c r="AC7" s="6">
-        <f t="shared" si="8"/>
-        <v>0.79107142857142854</v>
-      </c>
       <c r="AD7">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -2341,7 +2911,7 @@
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>10</v>
@@ -2353,10 +2923,10 @@
         <v>7</v>
       </c>
       <c r="E8" s="3">
-        <v>47.5</v>
+        <v>44.8</v>
       </c>
       <c r="F8" s="3">
-        <v>12.8</v>
+        <v>12.5</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="2">
@@ -2366,83 +2936,185 @@
         <v>6</v>
       </c>
       <c r="J8" s="2">
+        <v>16</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>95</v>
+      </c>
+      <c r="M8" s="2">
+        <v>134</v>
+      </c>
+      <c r="N8" s="2">
+        <v>34</v>
+      </c>
+      <c r="O8" s="2">
+        <v>443</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <f>99.6*65</f>
+        <v>6474</v>
+      </c>
+      <c r="S8" s="2">
+        <v>32</v>
+      </c>
+      <c r="T8" s="2">
+        <f>73958+14955</f>
+        <v>88913</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="1"/>
+        <v>279</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="2"/>
+        <v>443</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="3"/>
+        <v>1809600</v>
+      </c>
+      <c r="Y8" s="6">
+        <f t="shared" si="4"/>
+        <v>117.92175066312997</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="5"/>
+        <v>560</v>
+      </c>
+      <c r="AA8" s="6">
+        <f t="shared" si="6"/>
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="AB8" s="6">
+        <f t="shared" si="7"/>
+        <v>0.49821428571428572</v>
+      </c>
+      <c r="AC8" s="6">
+        <f t="shared" si="8"/>
+        <v>0.79107142857142854</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30">
+      <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3">
+        <v>47.5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12.8</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>6</v>
+      </c>
+      <c r="J9" s="2">
         <v>36</v>
       </c>
-      <c r="K8" s="2">
-        <v>0</v>
-      </c>
-      <c r="L8" s="2">
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
         <v>111</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M9" s="2">
         <v>129</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N9" s="2">
         <v>43</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O9" s="2">
         <v>483</v>
       </c>
-      <c r="P8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>0</v>
-      </c>
-      <c r="R8" s="2">
+      <c r="P9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2">
         <f>105*65</f>
         <v>6825</v>
       </c>
-      <c r="S8" s="2">
+      <c r="S9" s="2">
         <v>29</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T9" s="2">
         <f>88654+17827</f>
         <v>106481</v>
       </c>
-      <c r="U8">
+      <c r="U9">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="V8">
+      <c r="V9">
         <f t="shared" si="1"/>
         <v>319</v>
       </c>
-      <c r="W8">
+      <c r="W9">
         <f t="shared" si="2"/>
         <v>483</v>
       </c>
-      <c r="X8">
+      <c r="X9">
         <f t="shared" si="3"/>
         <v>1994400</v>
       </c>
-      <c r="Y8" s="6">
+      <c r="Y9" s="6">
         <f t="shared" si="4"/>
         <v>128.13598074608905</v>
       </c>
-      <c r="Z8">
+      <c r="Z9">
         <f t="shared" si="5"/>
         <v>608</v>
       </c>
-      <c r="AA8" s="6">
+      <c r="AA9" s="6">
         <f t="shared" si="6"/>
         <v>4.7697368421052634E-2</v>
       </c>
-      <c r="AB8" s="6">
+      <c r="AB9" s="6">
         <f t="shared" si="7"/>
         <v>0.52467105263157898</v>
       </c>
-      <c r="AC8" s="6">
+      <c r="AC9" s="6">
         <f t="shared" si="8"/>
         <v>0.79440789473684215</v>
       </c>
-      <c r="AD8">
+      <c r="AD9">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
-      <c r="Y10" s="6"/>
+    <row r="11" spans="1:30">
+      <c r="Y11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
removed a space in one unit cell
</commit_message>
<xml_diff>
--- a/BridgesLCA/data/Bridges.xlsx
+++ b/BridgesLCA/data/Bridges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julien.cravero\source\repos\BridgesLCA\BridgesLCA\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StefanoMerciai\Departier_repo\BridgesLCA\BridgesLCA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EFD877-7439-44F1-BDF8-7DB7DDF3A67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A89642F-F28C-4A37-9610-A28FABB4E930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5762E621-FB6B-4264-B807-B2B391FF7D72}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5762E621-FB6B-4264-B807-B2B391FF7D72}"/>
   </bookViews>
   <sheets>
     <sheet name="bridges_data" sheetId="3" r:id="rId1"/>
@@ -360,7 +360,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -791,12 +791,12 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -858,7 +858,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="5"/>
@@ -870,7 +870,7 @@
         <v>89</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>93</v>
@@ -879,7 +879,7 @@
         <v>95</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>98</v>
@@ -912,7 +912,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -974,7 +974,7 @@
         <v>78887</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>320000</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>445500</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>72881</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>44182</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>88913</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -1364,30 +1364,30 @@
       <selection activeCell="J2" sqref="A1:T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.75" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="5" customWidth="1"/>
-    <col min="4" max="4" width="18.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.875" style="2"/>
-    <col min="7" max="7" width="10.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.875" style="2"/>
+    <col min="1" max="1" width="33.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.85546875" style="2"/>
+    <col min="7" max="7" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>78887</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>320000</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>445500</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>72881</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>44182</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>88913</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -1888,312 +1888,312 @@
         <v>106481</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="5:7">
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="5:7">
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="5:7">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="5:7">
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="5:7">
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="5:7">
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="5:7">
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="5:7">
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="5:7">
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="5:7">
+    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="5:7">
+    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="5:7">
+    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="5:7">
+    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="5:7">
+    <row r="30" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="5:7">
+    <row r="31" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="5:7">
+    <row r="32" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="5:7">
+    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="5:7">
+    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="5:7">
+    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="5:7">
+    <row r="36" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="5:7">
+    <row r="37" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="5:7">
+    <row r="38" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="5:7">
+    <row r="39" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="5:7">
+    <row r="40" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="5:7">
+    <row r="41" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="5:7">
+    <row r="42" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="5:7">
+    <row r="43" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="5:7">
+    <row r="44" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="5:7">
+    <row r="45" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="5:7">
+    <row r="46" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="5:7">
+    <row r="47" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="5:7">
+    <row r="48" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="5:7">
+    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="5:7">
+    <row r="50" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="5:7">
+    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
     </row>
-    <row r="52" spans="5:7">
+    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="5:7">
+    <row r="53" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
     </row>
-    <row r="54" spans="5:7">
+    <row r="54" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
     </row>
-    <row r="55" spans="5:7">
+    <row r="55" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
     </row>
-    <row r="56" spans="5:7">
+    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
     </row>
-    <row r="57" spans="5:7">
+    <row r="57" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="5:7">
+    <row r="58" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
     </row>
-    <row r="59" spans="5:7">
+    <row r="59" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
     </row>
-    <row r="60" spans="5:7">
+    <row r="60" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
     </row>
-    <row r="61" spans="5:7">
+    <row r="61" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
     </row>
-    <row r="62" spans="5:7">
+    <row r="62" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
     </row>
-    <row r="63" spans="5:7">
+    <row r="63" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
     </row>
-    <row r="64" spans="5:7">
+    <row r="64" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="5:7">
+    <row r="65" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
     </row>
-    <row r="66" spans="5:7">
+    <row r="66" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
     </row>
-    <row r="67" spans="5:7">
+    <row r="67" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
     </row>
-    <row r="68" spans="5:7">
+    <row r="68" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
     </row>
-    <row r="69" spans="5:7">
+    <row r="69" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
     </row>
-    <row r="70" spans="5:7">
+    <row r="70" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -2214,31 +2214,31 @@
       <selection activeCell="T9" sqref="A1:T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="37.75" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.25" customWidth="1"/>
-    <col min="25" max="25" width="29.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.28515625" customWidth="1"/>
+    <col min="25" max="25" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="5"/>
@@ -2394,7 +2394,7 @@
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:30" s="19" customFormat="1">
+    <row r="5" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>212.21590909090909</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="12" customFormat="1">
+    <row r="7" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="Y11" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new long bridges
</commit_message>
<xml_diff>
--- a/BridgesLCA/data/Bridges.xlsx
+++ b/BridgesLCA/data/Bridges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julien.cravero\source\repos\BridgesLCA\BridgesLCA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F72027-F286-4070-88CC-50C51E4FB697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43ECDD11-B9C5-4D92-BD01-4104C9253433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5762E621-FB6B-4264-B807-B2B391FF7D72}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -354,6 +354,36 @@
   </si>
   <si>
     <t>Concrete for Railings C30</t>
+  </si>
+  <si>
+    <t>Design BDRR</t>
+  </si>
+  <si>
+    <t>Chanteloup</t>
+  </si>
+  <si>
+    <t>Design SSA</t>
+  </si>
+  <si>
+    <t>Extradosed Prestressed Concrete</t>
+  </si>
+  <si>
+    <t>Design RD30</t>
+  </si>
+  <si>
+    <t>Achères-sur-Seine</t>
+  </si>
+  <si>
+    <t>Design RD190</t>
+  </si>
+  <si>
+    <t>Design Carrières</t>
+  </si>
+  <si>
+    <t>Carrières</t>
+  </si>
+  <si>
+    <t>Cantilever Prestressed Concrete</t>
   </si>
 </sst>
 </file>
@@ -791,14 +821,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10924730-7B98-45F4-B23C-B5F7ED65DD7F}">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
+    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.875" bestFit="1" customWidth="1"/>
@@ -888,7 +921,7 @@
         <v>89</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>93</v>
@@ -1367,6 +1400,321 @@
       <c r="T9" s="2">
         <f>88654+17827</f>
         <v>106481</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="2">
+        <v>78</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="3">
+        <v>680</v>
+      </c>
+      <c r="F10" s="3">
+        <v>26.96</v>
+      </c>
+      <c r="G10" s="2">
+        <v>20</v>
+      </c>
+      <c r="H10" s="2">
+        <v>12</v>
+      </c>
+      <c r="J10" s="2">
+        <v>2213</v>
+      </c>
+      <c r="K10" s="2">
+        <v>706950</v>
+      </c>
+      <c r="L10" s="2">
+        <v>2500</v>
+      </c>
+      <c r="M10" s="2">
+        <v>110</v>
+      </c>
+      <c r="N10" s="2">
+        <v>2417</v>
+      </c>
+      <c r="O10" s="2">
+        <v>15393</v>
+      </c>
+      <c r="P10" s="2">
+        <v>476500</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2">
+        <f>E10*4*65</f>
+        <v>176800</v>
+      </c>
+      <c r="S10" s="2">
+        <f>(536+1940+300)*0.1</f>
+        <v>277.60000000000002</v>
+      </c>
+      <c r="T10" s="2">
+        <f>3584000+1.1*14608</f>
+        <v>3600068.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="2">
+        <v>78</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="3">
+        <v>632</v>
+      </c>
+      <c r="F11" s="3">
+        <v>26.14</v>
+      </c>
+      <c r="G11" s="2">
+        <v>20</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7</v>
+      </c>
+      <c r="J11" s="2">
+        <f>1767+82</f>
+        <v>1849</v>
+      </c>
+      <c r="K11" s="2">
+        <v>10600</v>
+      </c>
+      <c r="L11" s="2">
+        <v>3347</v>
+      </c>
+      <c r="M11" s="2">
+        <v>252</v>
+      </c>
+      <c r="N11" s="2">
+        <v>1185</v>
+      </c>
+      <c r="O11" s="2">
+        <f>12303+1399</f>
+        <v>13702</v>
+      </c>
+      <c r="P11" s="2">
+        <v>373560</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
+        <f>E11*4*65</f>
+        <v>164320</v>
+      </c>
+      <c r="S11" s="2">
+        <f>117.8*0.1</f>
+        <v>11.780000000000001</v>
+      </c>
+      <c r="T11" s="2">
+        <v>3017907</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="2">
+        <v>78</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="3">
+        <v>612</v>
+      </c>
+      <c r="F12" s="3">
+        <v>27.17</v>
+      </c>
+      <c r="G12" s="2">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="H12" s="2">
+        <v>4</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1600</v>
+      </c>
+      <c r="K12" s="2">
+        <f>438633+44647</f>
+        <v>483280</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M12" s="2">
+        <v>796.5</v>
+      </c>
+      <c r="N12" s="2">
+        <v>1030</v>
+      </c>
+      <c r="O12" s="2">
+        <f>10998+81.5+404</f>
+        <v>11483.5</v>
+      </c>
+      <c r="P12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2">
+        <f t="shared" ref="R12:R14" si="0">E12*4*65</f>
+        <v>159120</v>
+      </c>
+      <c r="S12" s="2">
+        <f>3000*0.1</f>
+        <v>300</v>
+      </c>
+      <c r="T12" s="2">
+        <v>2413281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="2">
+        <v>78</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="3">
+        <v>621</v>
+      </c>
+      <c r="F13" s="3">
+        <v>26.45</v>
+      </c>
+      <c r="G13" s="2">
+        <v>20</v>
+      </c>
+      <c r="H13" s="2">
+        <v>7</v>
+      </c>
+      <c r="J13" s="2">
+        <f>992+4285/2.5</f>
+        <v>2706</v>
+      </c>
+      <c r="K13" s="2">
+        <v>185000</v>
+      </c>
+      <c r="L13" s="2">
+        <v>2093</v>
+      </c>
+      <c r="M13" s="2">
+        <v>500</v>
+      </c>
+      <c r="N13" s="2">
+        <v>2023</v>
+      </c>
+      <c r="O13" s="2">
+        <f>12649+370</f>
+        <v>13019</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2">
+        <f t="shared" si="0"/>
+        <v>161460</v>
+      </c>
+      <c r="S13" s="2">
+        <f>1221*0.1</f>
+        <v>122.10000000000001</v>
+      </c>
+      <c r="T13" s="2">
+        <v>2173380</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="2">
+        <v>78</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="3">
+        <v>590</v>
+      </c>
+      <c r="F14" s="3">
+        <v>24.34</v>
+      </c>
+      <c r="G14" s="2">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="H14" s="2">
+        <v>8</v>
+      </c>
+      <c r="J14" s="2">
+        <f>8200+2400</f>
+        <v>10600</v>
+      </c>
+      <c r="K14" s="2">
+        <v>550000</v>
+      </c>
+      <c r="L14" s="2">
+        <v>5173</v>
+      </c>
+      <c r="M14" s="2">
+        <f>1000+40</f>
+        <v>1040</v>
+      </c>
+      <c r="N14" s="2">
+        <v>912</v>
+      </c>
+      <c r="O14" s="2">
+        <f>12085+690</f>
+        <v>12775</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
+        <f t="shared" si="0"/>
+        <v>153400</v>
+      </c>
+      <c r="S14" s="2">
+        <f>1284*0.1</f>
+        <v>128.4</v>
+      </c>
+      <c r="T14" s="2">
+        <v>2998000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"changed the excel file"
</commit_message>
<xml_diff>
--- a/BridgesLCA/data/Bridges.xlsx
+++ b/BridgesLCA/data/Bridges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julien.cravero\source\repos\BridgesLCA\BridgesLCA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43ECDD11-B9C5-4D92-BD01-4104C9253433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570CC157-DC06-426C-A396-AFBB2FADD97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5762E621-FB6B-4264-B807-B2B391FF7D72}"/>
   </bookViews>
@@ -824,7 +824,7 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
no apparent changes but still
</commit_message>
<xml_diff>
--- a/BridgesLCA/data/Bridges.xlsx
+++ b/BridgesLCA/data/Bridges.xlsx
@@ -381,8 +381,8 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
-    <numFmt numFmtId="168" formatCode="General"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -467,91 +467,91 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -806,897 +806,897 @@
   </sheetPr>
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="25.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="33.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="19.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="33.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="19.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="20.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="23.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="23.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="19.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="3" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="6" t="n">
         <v>44</v>
       </c>
-      <c r="F3" s="5" t="n">
+      <c r="F3" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="G3" s="6" t="n">
         <v>7.8</v>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="J3" s="3" t="n">
+      <c r="J3" s="4" t="n">
         <v>85</v>
       </c>
-      <c r="K3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3" t="n">
+      <c r="K3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4" t="n">
         <v>149</v>
       </c>
-      <c r="M3" s="3" t="n">
+      <c r="M3" s="4" t="n">
         <v>54</v>
       </c>
-      <c r="N3" s="3" t="n">
+      <c r="N3" s="4" t="n">
         <v>200</v>
       </c>
-      <c r="O3" s="3" t="n">
+      <c r="O3" s="4" t="n">
         <v>283</v>
       </c>
-      <c r="P3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" s="3" t="n">
+      <c r="P3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="4" t="n">
         <v>12090</v>
       </c>
-      <c r="S3" s="3" t="n">
+      <c r="S3" s="4" t="n">
         <v>185</v>
       </c>
-      <c r="T3" s="3" t="n">
+      <c r="T3" s="4" t="n">
         <v>78887</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="6" t="n">
         <v>46</v>
       </c>
-      <c r="F4" s="5" t="n">
+      <c r="F4" s="6" t="n">
         <v>36</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="J4" s="4" t="n">
         <v>202</v>
       </c>
-      <c r="K4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3" t="n">
+      <c r="K4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4" t="n">
         <v>596</v>
       </c>
-      <c r="M4" s="3" t="n">
+      <c r="M4" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="N4" s="3" t="n">
+      <c r="N4" s="4" t="n">
         <v>300</v>
       </c>
-      <c r="O4" s="3" t="n">
+      <c r="O4" s="4" t="n">
         <v>1230</v>
       </c>
-      <c r="P4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" s="3" t="n">
+      <c r="P4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="4" t="n">
         <f aca="false">99.6*65</f>
         <v>6474</v>
       </c>
-      <c r="S4" s="3" t="n">
+      <c r="S4" s="4" t="n">
         <v>202</v>
       </c>
-      <c r="T4" s="3" t="n">
+      <c r="T4" s="4" t="n">
         <f aca="false">276000+44000</f>
         <v>320000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="9" t="n">
+      <c r="E5" s="10" t="n">
         <v>80</v>
       </c>
-      <c r="F5" s="9" t="n">
+      <c r="F5" s="10" t="n">
         <v>22</v>
       </c>
-      <c r="G5" s="9" t="n">
+      <c r="G5" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="H5" s="10" t="n">
+      <c r="H5" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="I5" s="10" t="n">
+      <c r="I5" s="11" t="n">
         <v>19</v>
       </c>
-      <c r="J5" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="10" t="n">
+      <c r="J5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="11" t="n">
         <v>135700</v>
       </c>
-      <c r="L5" s="10" t="n">
+      <c r="L5" s="11" t="n">
         <v>711</v>
       </c>
-      <c r="M5" s="10" t="n">
+      <c r="M5" s="11" t="n">
         <v>129</v>
       </c>
-      <c r="N5" s="10" t="n">
+      <c r="N5" s="11" t="n">
         <v>773</v>
       </c>
-      <c r="O5" s="10" t="n">
+      <c r="O5" s="11" t="n">
         <v>864</v>
       </c>
-      <c r="P5" s="10" t="n">
+      <c r="P5" s="11" t="n">
         <v>373500</v>
       </c>
-      <c r="Q5" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" s="10" t="n">
+      <c r="Q5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="11" t="n">
         <v>19000</v>
       </c>
-      <c r="S5" s="10" t="n">
+      <c r="S5" s="11" t="n">
         <v>604</v>
       </c>
-      <c r="T5" s="10" t="n">
+      <c r="T5" s="11" t="n">
         <f aca="false">175000+110000+160500</f>
         <v>445500</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="6" t="n">
         <v>51.5</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="F6" s="6" t="n">
         <v>9.6</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="H6" s="3" t="n">
+      <c r="H6" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="I6" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="J6" s="3" t="n">
+      <c r="J6" s="4" t="n">
         <v>119</v>
       </c>
-      <c r="K6" s="3" t="n">
+      <c r="K6" s="4" t="n">
         <f aca="false">2731+428</f>
         <v>3159</v>
       </c>
-      <c r="L6" s="3" t="n">
+      <c r="L6" s="4" t="n">
         <v>70</v>
       </c>
-      <c r="M6" s="3" t="n">
+      <c r="M6" s="4" t="n">
         <v>188</v>
       </c>
-      <c r="N6" s="3" t="n">
+      <c r="N6" s="4" t="n">
         <v>63</v>
       </c>
-      <c r="O6" s="3" t="n">
+      <c r="O6" s="4" t="n">
         <v>365</v>
       </c>
-      <c r="P6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="3" t="n">
+      <c r="P6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="R6" s="3" t="n">
+      <c r="R6" s="4" t="n">
         <f aca="false">136*65</f>
         <v>8840</v>
       </c>
-      <c r="S6" s="3" t="n">
+      <c r="S6" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="T6" s="3" t="n">
+      <c r="T6" s="4" t="n">
         <f aca="false">14165+57050+1666</f>
         <v>72881</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="14" t="n">
+      <c r="E7" s="15" t="n">
         <v>7.7</v>
       </c>
-      <c r="F7" s="14" t="n">
+      <c r="F7" s="15" t="n">
         <v>16.2</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15" t="n">
+      <c r="G7" s="15"/>
+      <c r="H7" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="15" t="n">
+      <c r="I7" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="J7" s="15" t="n">
+      <c r="J7" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="K7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="15" t="n">
+      <c r="K7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="16" t="n">
         <v>66</v>
       </c>
-      <c r="M7" s="15" t="n">
+      <c r="M7" s="16" t="n">
         <v>34</v>
       </c>
-      <c r="N7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" s="15" t="n">
+      <c r="N7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="16" t="n">
         <v>151</v>
       </c>
-      <c r="P7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" s="15" t="n">
+      <c r="P7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="16" t="n">
         <f aca="false">27*65</f>
         <v>1755</v>
       </c>
-      <c r="S7" s="15" t="n">
+      <c r="S7" s="16" t="n">
         <v>24</v>
       </c>
-      <c r="T7" s="15" t="n">
+      <c r="T7" s="16" t="n">
         <v>44182</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="6" t="n">
         <v>44.8</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="6" t="n">
         <v>12.5</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="3" t="n">
+      <c r="G8" s="6"/>
+      <c r="H8" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="I8" s="3" t="n">
+      <c r="I8" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="J8" s="3" t="n">
+      <c r="J8" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="K8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3" t="n">
+      <c r="K8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4" t="n">
         <v>95</v>
       </c>
-      <c r="M8" s="3" t="n">
+      <c r="M8" s="4" t="n">
         <v>134</v>
       </c>
-      <c r="N8" s="3" t="n">
+      <c r="N8" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="O8" s="3" t="n">
+      <c r="O8" s="4" t="n">
         <v>443</v>
       </c>
-      <c r="P8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" s="3" t="n">
+      <c r="P8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="4" t="n">
         <f aca="false">99.6*65</f>
         <v>6474</v>
       </c>
-      <c r="S8" s="3" t="n">
+      <c r="S8" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="T8" s="3" t="n">
+      <c r="T8" s="4" t="n">
         <f aca="false">73958+14955</f>
         <v>88913</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="6" t="n">
         <v>47.5</v>
       </c>
-      <c r="F9" s="5" t="n">
+      <c r="F9" s="6" t="n">
         <v>12.8</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="3" t="n">
+      <c r="G9" s="6"/>
+      <c r="H9" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="I9" s="3" t="n">
+      <c r="I9" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="J9" s="3" t="n">
+      <c r="J9" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="K9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3" t="n">
+      <c r="K9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4" t="n">
         <v>111</v>
       </c>
-      <c r="M9" s="3" t="n">
+      <c r="M9" s="4" t="n">
         <v>129</v>
       </c>
-      <c r="N9" s="3" t="n">
+      <c r="N9" s="4" t="n">
         <v>43</v>
       </c>
-      <c r="O9" s="3" t="n">
+      <c r="O9" s="4" t="n">
         <v>483</v>
       </c>
-      <c r="P9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" s="3" t="n">
+      <c r="P9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="4" t="n">
         <f aca="false">105*65</f>
         <v>6825</v>
       </c>
-      <c r="S9" s="3" t="n">
+      <c r="S9" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="T9" s="3" t="n">
+      <c r="T9" s="4" t="n">
         <f aca="false">88654+17827</f>
         <v>106481</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="4" t="n">
         <v>78</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="5" t="n">
+      <c r="E10" s="6" t="n">
         <v>680</v>
       </c>
-      <c r="F10" s="5" t="n">
+      <c r="F10" s="6" t="n">
         <v>26.96</v>
       </c>
-      <c r="G10" s="3" t="n">
+      <c r="G10" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="H10" s="3" t="n">
+      <c r="H10" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="J10" s="3" t="n">
+      <c r="J10" s="4" t="n">
         <v>2213</v>
       </c>
-      <c r="K10" s="3" t="n">
+      <c r="K10" s="4" t="n">
         <v>706950</v>
       </c>
-      <c r="L10" s="3" t="n">
+      <c r="L10" s="4" t="n">
         <v>2500</v>
       </c>
-      <c r="M10" s="3" t="n">
+      <c r="M10" s="4" t="n">
         <v>110</v>
       </c>
-      <c r="N10" s="3" t="n">
+      <c r="N10" s="4" t="n">
         <v>2417</v>
       </c>
-      <c r="O10" s="3" t="n">
+      <c r="O10" s="4" t="n">
         <v>15393</v>
       </c>
-      <c r="P10" s="3" t="n">
+      <c r="P10" s="4" t="n">
         <v>476500</v>
       </c>
-      <c r="Q10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R10" s="3" t="n">
+      <c r="Q10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" s="4" t="n">
         <f aca="false">E10*4*65</f>
         <v>176800</v>
       </c>
-      <c r="S10" s="3" t="n">
+      <c r="S10" s="4" t="n">
         <f aca="false">(536+1940+300)*0.1</f>
         <v>277.6</v>
       </c>
-      <c r="T10" s="3" t="n">
+      <c r="T10" s="4" t="n">
         <f aca="false">3584000+1.1*14608</f>
         <v>3600068.8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="4" t="n">
         <v>78</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="5" t="n">
+      <c r="E11" s="6" t="n">
         <v>632</v>
       </c>
-      <c r="F11" s="5" t="n">
+      <c r="F11" s="6" t="n">
         <v>26.14</v>
       </c>
-      <c r="G11" s="3" t="n">
+      <c r="G11" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="H11" s="3" t="n">
+      <c r="H11" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="J11" s="3" t="n">
+      <c r="J11" s="4" t="n">
         <f aca="false">1767+82</f>
         <v>1849</v>
       </c>
-      <c r="K11" s="3" t="n">
+      <c r="K11" s="4" t="n">
         <v>10600</v>
       </c>
-      <c r="L11" s="3" t="n">
+      <c r="L11" s="4" t="n">
         <v>3347</v>
       </c>
-      <c r="M11" s="3" t="n">
+      <c r="M11" s="4" t="n">
         <v>252</v>
       </c>
-      <c r="N11" s="3" t="n">
+      <c r="N11" s="4" t="n">
         <v>1185</v>
       </c>
-      <c r="O11" s="3" t="n">
+      <c r="O11" s="4" t="n">
         <f aca="false">12303+1399</f>
         <v>13702</v>
       </c>
-      <c r="P11" s="3" t="n">
+      <c r="P11" s="4" t="n">
         <v>373560</v>
       </c>
-      <c r="Q11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" s="3" t="n">
+      <c r="Q11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="4" t="n">
         <f aca="false">E11*4*65</f>
         <v>164320</v>
       </c>
-      <c r="S11" s="3" t="n">
+      <c r="S11" s="4" t="n">
         <f aca="false">117.8*0.1</f>
         <v>11.78</v>
       </c>
-      <c r="T11" s="3" t="n">
+      <c r="T11" s="4" t="n">
         <v>3017907</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="4" t="n">
         <v>78</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="5" t="n">
+      <c r="E12" s="6" t="n">
         <v>612</v>
       </c>
-      <c r="F12" s="5" t="n">
+      <c r="F12" s="6" t="n">
         <v>27.17</v>
       </c>
-      <c r="G12" s="3" t="n">
+      <c r="G12" s="4" t="n">
         <v>17.1</v>
       </c>
-      <c r="H12" s="3" t="n">
+      <c r="H12" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="J12" s="3" t="n">
+      <c r="J12" s="4" t="n">
         <v>1600</v>
       </c>
-      <c r="K12" s="3" t="n">
+      <c r="K12" s="4" t="n">
         <f aca="false">438633+44647</f>
         <v>483280</v>
       </c>
-      <c r="L12" s="3" t="n">
+      <c r="L12" s="4" t="n">
         <v>1000</v>
       </c>
-      <c r="M12" s="3" t="n">
+      <c r="M12" s="4" t="n">
         <v>796.5</v>
       </c>
-      <c r="N12" s="3" t="n">
+      <c r="N12" s="4" t="n">
         <v>1030</v>
       </c>
-      <c r="O12" s="3" t="n">
+      <c r="O12" s="4" t="n">
         <f aca="false">10998+81.5+404</f>
         <v>11483.5</v>
       </c>
-      <c r="P12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" s="3" t="n">
+      <c r="P12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="4" t="n">
         <f aca="false">E12*4*65</f>
         <v>159120</v>
       </c>
-      <c r="S12" s="3" t="n">
+      <c r="S12" s="4" t="n">
         <f aca="false">3000*0.1</f>
         <v>300</v>
       </c>
-      <c r="T12" s="3" t="n">
+      <c r="T12" s="4" t="n">
         <v>2413281</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="3" t="n">
+      <c r="C13" s="4" t="n">
         <v>78</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="5" t="n">
+      <c r="E13" s="6" t="n">
         <v>621</v>
       </c>
-      <c r="F13" s="5" t="n">
+      <c r="F13" s="6" t="n">
         <v>26.45</v>
       </c>
-      <c r="G13" s="3" t="n">
+      <c r="G13" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="H13" s="3" t="n">
+      <c r="H13" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="J13" s="3" t="n">
+      <c r="J13" s="4" t="n">
         <f aca="false">992+4285/2.5</f>
         <v>2706</v>
       </c>
-      <c r="K13" s="3" t="n">
+      <c r="K13" s="4" t="n">
         <v>185000</v>
       </c>
-      <c r="L13" s="3" t="n">
+      <c r="L13" s="4" t="n">
         <v>2093</v>
       </c>
-      <c r="M13" s="3" t="n">
+      <c r="M13" s="4" t="n">
         <v>500</v>
       </c>
-      <c r="N13" s="3" t="n">
+      <c r="N13" s="4" t="n">
         <v>2023</v>
       </c>
-      <c r="O13" s="3" t="n">
+      <c r="O13" s="4" t="n">
         <f aca="false">12649+370</f>
         <v>13019</v>
       </c>
-      <c r="P13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" s="3" t="n">
+      <c r="P13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="4" t="n">
         <f aca="false">E13*4*65</f>
         <v>161460</v>
       </c>
-      <c r="S13" s="3" t="n">
+      <c r="S13" s="4" t="n">
         <f aca="false">1221*0.1</f>
         <v>122.1</v>
       </c>
-      <c r="T13" s="3" t="n">
+      <c r="T13" s="4" t="n">
         <v>2173380</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="4" t="n">
         <v>78</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="5" t="n">
+      <c r="E14" s="6" t="n">
         <v>590</v>
       </c>
-      <c r="F14" s="5" t="n">
+      <c r="F14" s="6" t="n">
         <v>24.34</v>
       </c>
-      <c r="G14" s="3" t="n">
+      <c r="G14" s="4" t="n">
         <v>18.1</v>
       </c>
-      <c r="H14" s="3" t="n">
+      <c r="H14" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="J14" s="3" t="n">
+      <c r="J14" s="4" t="n">
         <f aca="false">8200+2400</f>
         <v>10600</v>
       </c>
-      <c r="K14" s="3" t="n">
+      <c r="K14" s="4" t="n">
         <v>550000</v>
       </c>
-      <c r="L14" s="3" t="n">
+      <c r="L14" s="4" t="n">
         <v>5173</v>
       </c>
-      <c r="M14" s="3" t="n">
+      <c r="M14" s="4" t="n">
         <f aca="false">1000+40</f>
         <v>1040</v>
       </c>
-      <c r="N14" s="3" t="n">
+      <c r="N14" s="4" t="n">
         <v>912</v>
       </c>
-      <c r="O14" s="3" t="n">
+      <c r="O14" s="4" t="n">
         <f aca="false">12085+690</f>
         <v>12775</v>
       </c>
-      <c r="P14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" s="3" t="n">
+      <c r="P14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" s="4" t="n">
         <f aca="false">E14*4*65</f>
         <v>153400</v>
       </c>
-      <c r="S14" s="3" t="n">
+      <c r="S14" s="4" t="n">
         <f aca="false">1284*0.1</f>
         <v>128.4</v>
       </c>
-      <c r="T14" s="3" t="n">
+      <c r="T14" s="4" t="n">
         <v>2998000</v>
       </c>
     </row>
@@ -1724,837 +1724,837 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="33.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="24.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="3" width="8.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="10.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="19.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="25.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="23.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="24.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="32.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="3" width="15.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="17.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="22.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="3" width="15.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="3" width="24.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="21" style="3" width="8.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="33.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="24.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="18.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="4" width="8.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="10.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="19.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="25.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="23.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="32.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="4" width="15.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="4" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="4" width="17.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="4" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="4" width="15.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="4" width="24.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="21" style="4" width="8.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" s="6" t="n">
         <v>44</v>
       </c>
-      <c r="F2" s="5" t="n">
+      <c r="F2" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="G2" s="5" t="n">
+      <c r="G2" s="6" t="n">
         <v>7.8</v>
       </c>
-      <c r="H2" s="3" t="n">
+      <c r="H2" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="P2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" s="3" t="n">
+      <c r="P2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" s="4" t="n">
         <v>12090</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="T2" s="3" t="n">
+      <c r="T2" s="4" t="n">
         <v>78887</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="6" t="n">
         <v>46</v>
       </c>
-      <c r="F3" s="5" t="n">
+      <c r="F3" s="6" t="n">
         <v>36</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="G3" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="K3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3" t="s">
+      <c r="K3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" s="3" t="n">
+      <c r="P3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="4" t="n">
         <f aca="false">99.6*65</f>
         <v>6474</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="T3" s="3" t="n">
+      <c r="T3" s="4" t="n">
         <f aca="false">276000+44000</f>
         <v>320000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="6" t="n">
         <v>80</v>
       </c>
-      <c r="F4" s="5" t="n">
+      <c r="F4" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="J4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3" t="n">
+      <c r="J4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4" t="n">
         <v>135700</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="P4" s="3" t="n">
+      <c r="P4" s="4" t="n">
         <v>373500</v>
       </c>
-      <c r="Q4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" s="3" t="n">
+      <c r="Q4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="4" t="n">
         <v>19000</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="S4" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="T4" s="3" t="n">
+      <c r="T4" s="4" t="n">
         <f aca="false">175000+110000+160500</f>
         <v>445500</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="6" t="n">
         <v>51.5</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="6" t="n">
         <v>9.6</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="H5" s="3" t="n">
+      <c r="H5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="I5" s="3" t="n">
+      <c r="I5" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K5" s="3" t="n">
+      <c r="K5" s="4" t="n">
         <f aca="false">2731+428</f>
         <v>3159</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="P5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="3" t="s">
+      <c r="P5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="R5" s="3" t="n">
+      <c r="R5" s="4" t="n">
         <f aca="false">136*65</f>
         <v>8840</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="S5" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="T5" s="3" t="n">
+      <c r="T5" s="4" t="n">
         <f aca="false">14165+57050+1666</f>
         <v>72881</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="6" t="n">
         <v>7.7</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="F6" s="6" t="n">
         <v>16.2</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="3" t="n">
+      <c r="G6" s="6"/>
+      <c r="H6" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="I6" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" s="3" t="s">
+      <c r="K6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="N6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" s="3" t="s">
+      <c r="N6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="P6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="3" t="n">
+      <c r="P6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="4" t="n">
         <f aca="false">27*65</f>
         <v>1755</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="S6" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="T6" s="3" t="n">
+      <c r="T6" s="4" t="n">
         <v>44182</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="6" t="n">
         <v>44.8</v>
       </c>
-      <c r="F7" s="5" t="n">
+      <c r="F7" s="6" t="n">
         <v>12.5</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="3" t="n">
+      <c r="G7" s="6"/>
+      <c r="H7" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="K7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3" t="s">
+      <c r="K7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="P7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" s="3" t="n">
+      <c r="P7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="4" t="n">
         <f aca="false">99.6*65</f>
         <v>6474</v>
       </c>
-      <c r="S7" s="3" t="s">
+      <c r="S7" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="T7" s="3" t="n">
+      <c r="T7" s="4" t="n">
         <f aca="false">73958+14955</f>
         <v>88913</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="6" t="n">
         <v>47.5</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="6" t="n">
         <v>12.8</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="3" t="n">
+      <c r="G8" s="6"/>
+      <c r="H8" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="I8" s="3" t="n">
+      <c r="I8" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="K8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3" t="s">
+      <c r="K8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="P8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" s="3" t="n">
+      <c r="P8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="4" t="n">
         <f aca="false">105*65</f>
         <v>6825</v>
       </c>
-      <c r="S8" s="3" t="s">
+      <c r="S8" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="T8" s="3" t="n">
+      <c r="T8" s="4" t="n">
         <f aca="false">88654+17827</f>
         <v>106481</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2580,258 +2580,258 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="29.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="37.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="19.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="25.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="4.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="4.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="19.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="29.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="24.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="29.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="37.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="19.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="20.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="23.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="23.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="25.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="4.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="1" width="4.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="19.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="29.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="4" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="3" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="6" t="n">
         <v>44</v>
       </c>
-      <c r="F3" s="5" t="n">
+      <c r="F3" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="G3" s="6" t="n">
         <v>7.8</v>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="J3" s="3" t="n">
+      <c r="J3" s="4" t="n">
         <v>85</v>
       </c>
-      <c r="K3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3" t="n">
+      <c r="K3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4" t="n">
         <v>149</v>
       </c>
-      <c r="M3" s="3" t="n">
+      <c r="M3" s="4" t="n">
         <v>54</v>
       </c>
-      <c r="N3" s="3" t="n">
+      <c r="N3" s="4" t="n">
         <v>200</v>
       </c>
-      <c r="O3" s="3" t="n">
+      <c r="O3" s="4" t="n">
         <v>283</v>
       </c>
-      <c r="P3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" s="3" t="n">
+      <c r="P3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="4" t="n">
         <v>12090</v>
       </c>
-      <c r="S3" s="3" t="n">
+      <c r="S3" s="4" t="n">
         <v>185</v>
       </c>
-      <c r="T3" s="3" t="n">
+      <c r="T3" s="4" t="n">
         <v>78887</v>
       </c>
-      <c r="U3" s="16" t="n">
+      <c r="U3" s="1" t="n">
         <f aca="false">S3</f>
         <v>185</v>
       </c>
-      <c r="V3" s="16" t="n">
+      <c r="V3" s="1" t="n">
         <f aca="false">J3+L3+M3+N3</f>
         <v>488</v>
       </c>
-      <c r="W3" s="16" t="n">
+      <c r="W3" s="1" t="n">
         <f aca="false">O3</f>
         <v>283</v>
       </c>
-      <c r="X3" s="16" t="n">
+      <c r="X3" s="1" t="n">
         <f aca="false">(U3+V3+W3)*2400</f>
         <v>2294400</v>
       </c>
@@ -2839,7 +2839,7 @@
         <f aca="false">2400*T3/X3</f>
         <v>82.5177824267782</v>
       </c>
-      <c r="Z3" s="16" t="n">
+      <c r="Z3" s="1" t="n">
         <f aca="false">E3*F3</f>
         <v>484</v>
       </c>
@@ -2855,87 +2855,87 @@
         <f aca="false">W3/Z3</f>
         <v>0.584710743801653</v>
       </c>
-      <c r="AD3" s="16" t="n">
+      <c r="AD3" s="1" t="n">
         <f aca="false">P3/Z3</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="6" t="n">
         <v>46</v>
       </c>
-      <c r="F4" s="5" t="n">
+      <c r="F4" s="6" t="n">
         <v>36</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="J4" s="4" t="n">
         <v>202</v>
       </c>
-      <c r="K4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3" t="n">
+      <c r="K4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4" t="n">
         <v>596</v>
       </c>
-      <c r="M4" s="3" t="n">
+      <c r="M4" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="N4" s="3" t="n">
+      <c r="N4" s="4" t="n">
         <v>300</v>
       </c>
-      <c r="O4" s="3" t="n">
+      <c r="O4" s="4" t="n">
         <v>1230</v>
       </c>
-      <c r="P4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" s="3" t="n">
+      <c r="P4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="4" t="n">
         <f aca="false">99.6*65</f>
         <v>6474</v>
       </c>
-      <c r="S4" s="3" t="n">
+      <c r="S4" s="4" t="n">
         <v>202</v>
       </c>
-      <c r="T4" s="3" t="n">
+      <c r="T4" s="4" t="n">
         <f aca="false">276000+44000</f>
         <v>320000</v>
       </c>
-      <c r="U4" s="16" t="n">
+      <c r="U4" s="1" t="n">
         <f aca="false">S4</f>
         <v>202</v>
       </c>
-      <c r="V4" s="16" t="n">
+      <c r="V4" s="1" t="n">
         <f aca="false">J4+L4+M4+N4</f>
         <v>1134</v>
       </c>
-      <c r="W4" s="16" t="n">
+      <c r="W4" s="1" t="n">
         <f aca="false">O4</f>
         <v>1230</v>
       </c>
-      <c r="X4" s="16" t="n">
+      <c r="X4" s="1" t="n">
         <f aca="false">(U4+V4+W4)*2400</f>
         <v>6158400</v>
       </c>
@@ -2943,7 +2943,7 @@
         <f aca="false">2400*T4/X4</f>
         <v>124.707716289945</v>
       </c>
-      <c r="Z4" s="16" t="n">
+      <c r="Z4" s="1" t="n">
         <f aca="false">E4*F4</f>
         <v>1656</v>
       </c>
@@ -2959,70 +2959,70 @@
         <f aca="false">W4/Z4</f>
         <v>0.742753623188406</v>
       </c>
-      <c r="AD4" s="16" t="n">
+      <c r="AD4" s="1" t="n">
         <f aca="false">P4/Z4</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" s="18" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="9" t="n">
+      <c r="E5" s="10" t="n">
         <v>80</v>
       </c>
-      <c r="F5" s="9" t="n">
+      <c r="F5" s="10" t="n">
         <v>22</v>
       </c>
-      <c r="G5" s="9" t="n">
+      <c r="G5" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="H5" s="10" t="n">
+      <c r="H5" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="I5" s="10" t="n">
+      <c r="I5" s="11" t="n">
         <v>19</v>
       </c>
-      <c r="J5" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="10" t="n">
+      <c r="J5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="11" t="n">
         <v>135700</v>
       </c>
-      <c r="L5" s="10" t="n">
+      <c r="L5" s="11" t="n">
         <v>711</v>
       </c>
-      <c r="M5" s="10" t="n">
+      <c r="M5" s="11" t="n">
         <v>129</v>
       </c>
-      <c r="N5" s="10" t="n">
+      <c r="N5" s="11" t="n">
         <v>773</v>
       </c>
-      <c r="O5" s="10" t="n">
+      <c r="O5" s="11" t="n">
         <v>864</v>
       </c>
-      <c r="P5" s="10" t="n">
+      <c r="P5" s="11" t="n">
         <v>373500</v>
       </c>
-      <c r="Q5" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" s="10" t="n">
+      <c r="Q5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="11" t="n">
         <v>19000</v>
       </c>
-      <c r="S5" s="10" t="n">
+      <c r="S5" s="11" t="n">
         <v>604</v>
       </c>
-      <c r="T5" s="10" t="n">
+      <c r="T5" s="11" t="n">
         <f aca="false">175000+110000+160500</f>
         <v>445500</v>
       </c>
@@ -3068,82 +3068,82 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="6" t="n">
         <v>51.5</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="F6" s="6" t="n">
         <v>9.6</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="H6" s="3" t="n">
+      <c r="H6" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="I6" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="J6" s="3" t="n">
+      <c r="J6" s="4" t="n">
         <v>119</v>
       </c>
-      <c r="K6" s="3" t="n">
+      <c r="K6" s="4" t="n">
         <f aca="false">2731+428</f>
         <v>3159</v>
       </c>
-      <c r="L6" s="3" t="n">
+      <c r="L6" s="4" t="n">
         <v>70</v>
       </c>
-      <c r="M6" s="3" t="n">
+      <c r="M6" s="4" t="n">
         <v>188</v>
       </c>
-      <c r="N6" s="3" t="n">
+      <c r="N6" s="4" t="n">
         <v>63</v>
       </c>
-      <c r="O6" s="3" t="n">
+      <c r="O6" s="4" t="n">
         <v>365</v>
       </c>
-      <c r="P6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="3" t="n">
+      <c r="P6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="R6" s="3" t="n">
+      <c r="R6" s="4" t="n">
         <f aca="false">136*65</f>
         <v>8840</v>
       </c>
-      <c r="S6" s="3" t="n">
+      <c r="S6" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="T6" s="3" t="n">
+      <c r="T6" s="4" t="n">
         <f aca="false">14165+57050+1666</f>
         <v>72881</v>
       </c>
-      <c r="U6" s="16" t="n">
+      <c r="U6" s="1" t="n">
         <f aca="false">S6</f>
         <v>37</v>
       </c>
-      <c r="V6" s="16" t="n">
+      <c r="V6" s="1" t="n">
         <f aca="false">J6+L6+M6+N6</f>
         <v>440</v>
       </c>
-      <c r="W6" s="16" t="n">
+      <c r="W6" s="1" t="n">
         <f aca="false">O6</f>
         <v>365</v>
       </c>
-      <c r="X6" s="16" t="n">
+      <c r="X6" s="1" t="n">
         <f aca="false">(U6+V6+W6)*2400</f>
         <v>2020800</v>
       </c>
@@ -3151,7 +3151,7 @@
         <f aca="false">2400*T6/X6</f>
         <v>86.5570071258907</v>
       </c>
-      <c r="Z6" s="16" t="n">
+      <c r="Z6" s="1" t="n">
         <f aca="false">E6*F6</f>
         <v>494.4</v>
       </c>
@@ -3167,69 +3167,69 @@
         <f aca="false">W6/Z6</f>
         <v>0.73826860841424</v>
       </c>
-      <c r="AD6" s="16" t="n">
+      <c r="AD6" s="1" t="n">
         <f aca="false">P6/Z6</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" s="21" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="14" t="n">
+      <c r="E7" s="15" t="n">
         <v>7.7</v>
       </c>
-      <c r="F7" s="14" t="n">
+      <c r="F7" s="15" t="n">
         <v>16.2</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15" t="n">
+      <c r="G7" s="15"/>
+      <c r="H7" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="15" t="n">
+      <c r="I7" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="J7" s="15" t="n">
+      <c r="J7" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="K7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="15" t="n">
+      <c r="K7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="16" t="n">
         <v>66</v>
       </c>
-      <c r="M7" s="15" t="n">
+      <c r="M7" s="16" t="n">
         <v>34</v>
       </c>
-      <c r="N7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" s="15" t="n">
+      <c r="N7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="16" t="n">
         <v>151</v>
       </c>
-      <c r="P7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" s="15" t="n">
+      <c r="P7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="16" t="n">
         <f aca="false">27*65</f>
         <v>1755</v>
       </c>
-      <c r="S7" s="15" t="n">
+      <c r="S7" s="16" t="n">
         <v>24</v>
       </c>
-      <c r="T7" s="15" t="n">
+      <c r="T7" s="16" t="n">
         <v>44182</v>
       </c>
       <c r="U7" s="21" t="n">
@@ -3274,79 +3274,79 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="6" t="n">
         <v>44.8</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="6" t="n">
         <v>12.5</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="3" t="n">
+      <c r="G8" s="6"/>
+      <c r="H8" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="I8" s="3" t="n">
+      <c r="I8" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="J8" s="3" t="n">
+      <c r="J8" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="K8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3" t="n">
+      <c r="K8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4" t="n">
         <v>95</v>
       </c>
-      <c r="M8" s="3" t="n">
+      <c r="M8" s="4" t="n">
         <v>134</v>
       </c>
-      <c r="N8" s="3" t="n">
+      <c r="N8" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="O8" s="3" t="n">
+      <c r="O8" s="4" t="n">
         <v>443</v>
       </c>
-      <c r="P8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" s="3" t="n">
+      <c r="P8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="4" t="n">
         <f aca="false">99.6*65</f>
         <v>6474</v>
       </c>
-      <c r="S8" s="3" t="n">
+      <c r="S8" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="T8" s="3" t="n">
+      <c r="T8" s="4" t="n">
         <f aca="false">73958+14955</f>
         <v>88913</v>
       </c>
-      <c r="U8" s="16" t="n">
+      <c r="U8" s="1" t="n">
         <f aca="false">S8</f>
         <v>32</v>
       </c>
-      <c r="V8" s="16" t="n">
+      <c r="V8" s="1" t="n">
         <f aca="false">J8+L8+M8+N8</f>
         <v>279</v>
       </c>
-      <c r="W8" s="16" t="n">
+      <c r="W8" s="1" t="n">
         <f aca="false">O8</f>
         <v>443</v>
       </c>
-      <c r="X8" s="16" t="n">
+      <c r="X8" s="1" t="n">
         <f aca="false">(U8+V8+W8)*2400</f>
         <v>1809600</v>
       </c>
@@ -3354,7 +3354,7 @@
         <f aca="false">2400*T8/X8</f>
         <v>117.92175066313</v>
       </c>
-      <c r="Z8" s="16" t="n">
+      <c r="Z8" s="1" t="n">
         <f aca="false">E8*F8</f>
         <v>560</v>
       </c>
@@ -3370,85 +3370,85 @@
         <f aca="false">W8/Z8</f>
         <v>0.791071428571429</v>
       </c>
-      <c r="AD8" s="16" t="n">
+      <c r="AD8" s="1" t="n">
         <f aca="false">P8/Z8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="6" t="n">
         <v>47.5</v>
       </c>
-      <c r="F9" s="5" t="n">
+      <c r="F9" s="6" t="n">
         <v>12.8</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="3" t="n">
+      <c r="G9" s="6"/>
+      <c r="H9" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="I9" s="3" t="n">
+      <c r="I9" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="J9" s="3" t="n">
+      <c r="J9" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="K9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3" t="n">
+      <c r="K9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4" t="n">
         <v>111</v>
       </c>
-      <c r="M9" s="3" t="n">
+      <c r="M9" s="4" t="n">
         <v>129</v>
       </c>
-      <c r="N9" s="3" t="n">
+      <c r="N9" s="4" t="n">
         <v>43</v>
       </c>
-      <c r="O9" s="3" t="n">
+      <c r="O9" s="4" t="n">
         <v>483</v>
       </c>
-      <c r="P9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" s="3" t="n">
+      <c r="P9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="4" t="n">
         <f aca="false">105*65</f>
         <v>6825</v>
       </c>
-      <c r="S9" s="3" t="n">
+      <c r="S9" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="T9" s="3" t="n">
+      <c r="T9" s="4" t="n">
         <f aca="false">88654+17827</f>
         <v>106481</v>
       </c>
-      <c r="U9" s="16" t="n">
+      <c r="U9" s="1" t="n">
         <f aca="false">S9</f>
         <v>29</v>
       </c>
-      <c r="V9" s="16" t="n">
+      <c r="V9" s="1" t="n">
         <f aca="false">J9+L9+M9+N9</f>
         <v>319</v>
       </c>
-      <c r="W9" s="16" t="n">
+      <c r="W9" s="1" t="n">
         <f aca="false">O9</f>
         <v>483</v>
       </c>
-      <c r="X9" s="16" t="n">
+      <c r="X9" s="1" t="n">
         <f aca="false">(U9+V9+W9)*2400</f>
         <v>1994400</v>
       </c>
@@ -3456,7 +3456,7 @@
         <f aca="false">2400*T9/X9</f>
         <v>128.135980746089</v>
       </c>
-      <c r="Z9" s="16" t="n">
+      <c r="Z9" s="1" t="n">
         <f aca="false">E9*F9</f>
         <v>608</v>
       </c>
@@ -3472,7 +3472,7 @@
         <f aca="false">W9/Z9</f>
         <v>0.794407894736842</v>
       </c>
-      <c r="AD9" s="16" t="n">
+      <c r="AD9" s="1" t="n">
         <f aca="false">P9/Z9</f>
         <v>0</v>
       </c>

</xml_diff>